<commit_message>
new xlsx file format
</commit_message>
<xml_diff>
--- a/scale-manager/HarpConfig.xlsx
+++ b/scale-manager/HarpConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="98" windowWidth="20250" windowHeight="9473"/>
+    <workbookView xWindow="120" yWindow="98" windowWidth="20250" windowHeight="9473" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Presets" sheetId="2" r:id="rId1"/>
@@ -498,16 +498,16 @@
     <t>On the Scales page, any non-blank entry in columns B through N indicates that the scale contains that interval.  That is, it is equivalent to place a "b2" or "x" or "*" in column C.</t>
   </si>
   <si>
-    <t>The transpose root note is named with Roland convention (C4 == MIDI note 60)</t>
-  </si>
-  <si>
     <t>Scales should have unique names; if there are more than one scale with the same name, the parser will chose the first one</t>
   </si>
   <si>
-    <t>Root note name should be capital letter followed by an optional sharp (#) and a required octave number (e.g. C4, F#3)</t>
-  </si>
-  <si>
     <t xml:space="preserve">The Scales sheet can have blank rows - however the parser stops reading the table after seeing more than 3 consecutive empty names in column A </t>
+  </si>
+  <si>
+    <t>The transpose root note is named with Yamaha convention (C3 == MIDI note 60)</t>
+  </si>
+  <si>
+    <t>Root note name should be capital letter followed by an optional sharp (#) and a required octave number (e.g. C2, F#3)</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -8046,8 +8046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8096,7 +8096,7 @@
     </row>
     <row r="10" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B10" s="86" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
@@ -8115,12 +8115,12 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B14" s="86" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B15" s="86" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
@@ -8141,7 +8141,7 @@
     </row>
     <row r="20" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B20" s="86" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
fix preset key label to match config file
</commit_message>
<xml_diff>
--- a/scale-manager/HarpConfig.xlsx
+++ b/scale-manager/HarpConfig.xlsx
@@ -1180,10 +1180,10 @@
   <dimension ref="A1:U252"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K36" sqref="K36"/>
+      <selection pane="bottomRight" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1470,7 +1470,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="78">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B26" s="74" t="s">
         <v>28</v>
@@ -1478,7 +1478,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="78">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B27" s="74" t="s">
         <v>29</v>
@@ -1486,7 +1486,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="78">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B28" s="74" t="s">
         <v>30</v>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="78">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B29" s="74" t="s">
         <v>31</v>
@@ -1502,7 +1502,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="78">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B30" s="74" t="s">
         <v>32</v>
@@ -1510,7 +1510,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="78">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B31" s="74" t="s">
         <v>33</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="78">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B32" s="74" t="s">
         <v>34</v>
@@ -1526,7 +1526,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="78">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B33" s="74" t="s">
         <v>35</v>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="78">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B34" s="74" t="s">
         <v>36</v>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="78">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B35" s="74" t="s">
         <v>37</v>
@@ -1550,7 +1550,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="78">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B36" s="74" t="s">
         <v>38</v>
@@ -1558,7 +1558,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="78">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B37" s="74" t="s">
         <v>40</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="78">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B38" s="74" t="s">
         <v>39</v>
@@ -1574,7 +1574,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="78">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B39" s="74" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
yet another set of pin changes - physical stripboard didnt line up as planned (had to shift the DIN connectors)
</commit_message>
<xml_diff>
--- a/scale-manager/HarpConfig.xlsx
+++ b/scale-manager/HarpConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="98" windowWidth="20250" windowHeight="9473"/>
+    <workbookView xWindow="120" yWindow="98" windowWidth="20250" windowHeight="9473" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Presets" sheetId="2" r:id="rId1"/>
@@ -492,9 +492,6 @@
     <t>On the Presets table, the Scale Name must match a corresponding scale named in the Scales table</t>
   </si>
   <si>
-    <t>The MIDI channel config on the Presets panel can be left blank (this defaults to channel 1)</t>
-  </si>
-  <si>
     <t>On the Scales page, any non-blank entry in columns B through N indicates that the scale contains that interval.  That is, it is equivalent to place a "b2" or "x" or "*" in column C.</t>
   </si>
   <si>
@@ -511,6 +508,9 @@
   </si>
   <si>
     <t>Bb-1</t>
+  </si>
+  <si>
+    <t>The MIDI channel config on the Presets panel can be left blank (it defaults to channel 1)</t>
   </si>
 </sst>
 </file>
@@ -1179,7 +1179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1252,7 +1252,7 @@
         <v>141</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>57</v>
@@ -8049,8 +8049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8099,7 +8099,7 @@
     </row>
     <row r="10" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B10" s="86" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
@@ -8118,17 +8118,17 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B14" s="86" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B15" s="86" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B16" s="86" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
@@ -8139,12 +8139,12 @@
     </row>
     <row r="19" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B19" s="86" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B20" s="86" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>